<commit_message>
Endring av filstruktur. Ny input fra S-området
</commit_message>
<xml_diff>
--- a/data/2022-03-14 data_faktisk_barnetillegg.xlsx
+++ b/data/2022-03-14 data_faktisk_barnetillegg.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://navno-my.sharepoint.com/personal/eirik_lamoy_nav_no/Documents/Documents/R-prosjekter/maxKG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{8929D8E1-C1B3-4581-B595-E202B1DC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13D723BB-08A6-4E9C-903B-44DB66DE4DB4}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{8929D8E1-C1B3-4581-B595-E202B1DC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F979F48-FB26-482E-9000-E47F986C3F99}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="855" windowWidth="21600" windowHeight="18375" activeTab="2" xr2:uid="{0F417289-FB9E-45FD-B570-C5A0E3CFEB4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0F417289-FB9E-45FD-B570-C5A0E3CFEB4B}"/>
   </bookViews>
   <sheets>
-    <sheet name="barnetillegg_per_ar" sheetId="1" r:id="rId1"/>
-    <sheet name="did_estimate" sheetId="2" r:id="rId2"/>
-    <sheet name="did_cluster" sheetId="3" r:id="rId3"/>
-    <sheet name="bt_arlig_data" sheetId="4" r:id="rId4"/>
+    <sheet name="oppdatert_modell" sheetId="5" r:id="rId1"/>
+    <sheet name="faktisk_bt" sheetId="6" r:id="rId2"/>
+    <sheet name="barnetillegg_per_ar" sheetId="1" r:id="rId3"/>
+    <sheet name="did_estimate" sheetId="2" r:id="rId4"/>
+    <sheet name="did_cluster" sheetId="3" r:id="rId5"/>
+    <sheet name="bt_arlig_data" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="24">
   <si>
     <t>gr</t>
   </si>
@@ -105,6 +109,9 @@
   </si>
   <si>
     <t>2021</t>
+  </si>
+  <si>
+    <t>utb_bt</t>
   </si>
 </sst>
 </file>
@@ -591,12 +598,21 @@
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - uthevingsfarge 1" xfId="1" xr:uid="{B1F15296-7D68-420F-8B62-8A40DEA15A5F}"/>
@@ -951,6 +967,722 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D052F5-0F0C-43A5-B252-3C73DE907C55}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-9.5000000000000001E-2</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2/C2</f>
+        <v>-13.571428571428571</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C3" s="4">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-0.14910000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E7" si="0">D3/C3</f>
+        <v>-16.384615384615383</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2018</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-0.19120000000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>-19.12</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2019</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.2233</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>-21.471153846153847</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.2475</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>-22.916666666666664</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.26640000000000003</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>-23.575221238938056</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2016</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-9.4799999999999995E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8/C8</f>
+        <v>-11.85</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.06E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-0.14560000000000001</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" ref="E9:E13" si="1">D9/C9</f>
+        <v>-13.735849056603774</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2018</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.14E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-0.18809999999999999</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>-16.5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2019</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-0.21629999999999999</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>-18.176470588235293</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>-0.2354</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>-19.295081967213115</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.25219999999999998</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>-19.858267716535433</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58A7486-D1C3-4D59-A1AA-F6721F482BE3}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2015</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.59227154983541108</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.53231286907565645</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2017</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.48333099586148459</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.453407001181935</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.41848403587113631</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.39518488139498231</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2021</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.38429605926228888</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2015</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.86040506366128466</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2016</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.74196127731433459</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2017</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.6420569123369767</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.56977996118388696</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.52653972498485035</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.49490989356469051</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.47273156774746228</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2015</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.64931920528611098</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>0</v>
+      </c>
+      <c r="B17" s="9">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.59468141685458009</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.54609167923204638</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>0</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2018</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.51882744978138029</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>0</v>
+      </c>
+      <c r="B20" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.48158147473268742</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.45548972685248229</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>0</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2021</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.44560559738939681</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9">
+        <v>2015</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.86040506366128466</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2016</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.74196127731433459</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2017</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.6420569123369767</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <v>2018</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.56977996118388696</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.52653972498485035</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2020</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.49490989356469051</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9">
+        <v>2021</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.47273156774746228</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C7CB4-4B75-4CED-8027-23B870C68563}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -1376,7 +2108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F8A3D6-CEEE-452A-B316-7E864C05E638}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -1816,12 +2548,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980AACBE-3B7F-4428-A31D-4417DC7F1A03}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2922261-9F08-4A6B-BBA5-84F8391443F1}">
   <dimension ref="A1:G13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Endringer i figurer mm. Omgjøre til SVG-format
</commit_message>
<xml_diff>
--- a/data/2022-03-14 data_faktisk_barnetillegg.xlsx
+++ b/data/2022-03-14 data_faktisk_barnetillegg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://navno-my.sharepoint.com/personal/eirik_lamoy_nav_no/Documents/Documents/R-prosjekter/maxKG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{8929D8E1-C1B3-4581-B595-E202B1DC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F979F48-FB26-482E-9000-E47F986C3F99}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{8929D8E1-C1B3-4581-B595-E202B1DC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692FD23F-B2D2-4FF7-8587-6F625CD46FA6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0F417289-FB9E-45FD-B570-C5A0E3CFEB4B}"/>
+    <workbookView xWindow="57705" yWindow="4200" windowWidth="21600" windowHeight="15600" xr2:uid="{0F417289-FB9E-45FD-B570-C5A0E3CFEB4B}"/>
   </bookViews>
   <sheets>
     <sheet name="oppdatert_modell" sheetId="5" r:id="rId1"/>
@@ -968,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D052F5-0F0C-43A5-B252-3C73DE907C55}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
     <col min="6" max="6" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1024,8 +1024,10 @@
       <c r="F2" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1045,8 +1047,10 @@
       <c r="F3" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1054,20 +1058,20 @@
         <v>2018</v>
       </c>
       <c r="C4" s="4">
-        <v>0.01</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="D4" s="3">
-        <v>-0.19120000000000001</v>
+        <v>-0.17910000000000001</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>-19.12</v>
+        <v>-18.852631578947371</v>
       </c>
       <c r="F4" s="3">
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1087,8 +1091,10 @@
       <c r="F5" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1108,8 +1114,10 @@
       <c r="F6" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1129,8 +1137,10 @@
       <c r="F7" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1150,8 +1160,10 @@
       <c r="F8" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1171,8 +1183,10 @@
       <c r="F9" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1183,17 +1197,19 @@
         <v>1.14E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.18809999999999999</v>
+        <v>-0.18509999999999999</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="1"/>
-        <v>-16.5</v>
+        <v>-16.236842105263158</v>
       </c>
       <c r="F10" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1213,8 +1229,10 @@
       <c r="F11" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1234,8 +1252,10 @@
       <c r="F12" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1255,6 +1275,8 @@
       <c r="F13" s="3">
         <v>0.9</v>
       </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1265,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58A7486-D1C3-4D59-A1AA-F6721F482BE3}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1716,7 @@
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2113,7 +2135,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>